<commit_message>
made a item code workbook
</commit_message>
<xml_diff>
--- a/scripts/rm_componentTests.xlsx
+++ b/scripts/rm_componentTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mat/Projects/Work/PDI/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAC2743-2BF4-734A-8010-D5DCCD62AC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C602C51-5FC2-2F43-BAFB-36E23BC6DC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2240" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestAndSpecs!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1538,10 +1546,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
   <dimension ref="A1:I219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="I221" sqref="I221"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>